<commit_message>
added some changes in html and css file
</commit_message>
<xml_diff>
--- a/your_excel_file.xlsx
+++ b/your_excel_file.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nirbhay Raj Mishra\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nirbhay Raj Mishra\Desktop\ExcelSearchApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1847,13 +1847,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2156,7 +2156,7 @@
   <dimension ref="A2:D572"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2179,12 +2179,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="28" t="s">
         <v>530</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
     </row>
     <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="25"/>
@@ -2193,16 +2193,16 @@
       <c r="D3" s="25"/>
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="26" t="s">
         <v>521</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="27" t="s">
         <v>522</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="27" t="s">
         <v>523</v>
       </c>
     </row>

</xml_diff>